<commit_message>
Updated code and BOM
Added code to check for a CRC to ensure data is correct.

Also changed the BOM to allow for a shorter controller design
</commit_message>
<xml_diff>
--- a/Motor Controller BOM.xlsx
+++ b/Motor Controller BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Desktop\Motor-Controller-main\Motor-Controller-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanson\Desktop\Motor-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEFE6AA-F6AA-4E83-882B-F2E0679AEB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59214C5C-B431-4548-A786-A62B548B6B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -244,15 +244,6 @@
     <t>https://www.infineon.com/dgdl/irfs3306pbf.pdf?fileId=5546d462533600a40153563682652165</t>
   </si>
   <si>
-    <t>175-MAX17640CATA+-ND</t>
-  </si>
-  <si>
-    <t>Buck Switching Regulator IC Positive Adjustable 0.9V 1 Output 400mA 8-WDFN</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/maxim-integrated/MAX17640CATA/14287861</t>
-  </si>
-  <si>
     <t>Q1-Q4</t>
   </si>
   <si>
@@ -295,15 +286,6 @@
     <t>CL32B226MOJVPNE Samsung Electro-Mechanics | Capacitors | DigiKey</t>
   </si>
   <si>
-    <t>1189-1505-ND</t>
-  </si>
-  <si>
-    <t>2200 µF 63 V Aluminum Electrolytic Capacitors Radial, Can - 10000 Hrs @ 105°C</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/rubycon/63ZLH2200MEFC18X40/3134461</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -338,6 +320,24 @@
   </si>
   <si>
     <t>Red, Yellow 630nm Red, 591nm Yellow LED Indication - Discrete 2V Red, 2V Yellow 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>175-MAX17640BATA+-ND</t>
+  </si>
+  <si>
+    <t>Buck Switching Regulator IC Positive Fixed 5V 1 Output 400mA 8-WFDFN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/maxim-integrated/MAX17640BATA/14287859?s=N4IgTCBcDaIIwHYCsBaAsgQQBqIGwBYAGAIQwBUMBqFAOQBEQBdAXyA</t>
+  </si>
+  <si>
+    <t>1189-4388-ND</t>
+  </si>
+  <si>
+    <t>2200 µF 50 V Aluminum Electrolytic Capacitors Radial, Can - 10000 Hrs @ 105°C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rubycon/50ZLJ2200M18X25/10437363</t>
   </si>
 </sst>
 </file>
@@ -945,22 +945,22 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="85.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -986,15 +986,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
@@ -1013,9 +1013,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>62</v>
@@ -1040,34 +1040,34 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D4" s="12">
         <v>2</v>
       </c>
       <c r="E4" s="19">
-        <v>2.92</v>
+        <v>2.84</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="19">
         <f t="shared" si="0"/>
-        <v>5.84</v>
+        <v>5.68</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
@@ -1094,9 +1094,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>51</v>
@@ -1121,15 +1121,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D7" s="20">
         <v>1</v>
@@ -1145,18 +1145,18 @@
         <v>0.37</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="C8" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D8" s="20">
         <v>1</v>
@@ -1172,18 +1172,18 @@
         <v>0.43</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D9" s="20">
         <v>2</v>
@@ -1199,12 +1199,12 @@
         <v>0.2</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>65</v>
@@ -1229,7 +1229,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
@@ -1257,15 +1257,15 @@
       </c>
       <c r="I11" s="17"/>
     </row>
-    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D12" s="20">
         <v>1</v>
@@ -1281,18 +1281,18 @@
         <v>1.65</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13" s="20">
         <v>1</v>
@@ -1308,18 +1308,18 @@
         <v>0.3</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="20">
         <v>1</v>
@@ -1335,12 +1335,12 @@
         <v>0.71</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>59</v>
@@ -1365,7 +1365,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>13</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>32</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>39</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>25</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="13" t="s">
         <v>24</v>
@@ -1552,9 +1552,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="35.4" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>40</v>
@@ -1579,7 +1579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>9</v>
       </c>
@@ -1606,65 +1606,65 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G25" s="7">
         <f>SUM(G2:G24)</f>
-        <v>59.519999999999989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59.359999999999992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1689,13 +1689,13 @@
     <hyperlink ref="H15" r:id="rId14" xr:uid="{28A63484-4740-4D85-A1B3-E119463E6BD6}"/>
     <hyperlink ref="H3" r:id="rId15" xr:uid="{FD5D0C32-AD08-46C3-BC7F-C3B51DF6FD14}"/>
     <hyperlink ref="H10" r:id="rId16" xr:uid="{E32EE017-42E4-4CF2-9F0F-93BCABEB36A9}"/>
-    <hyperlink ref="H12" r:id="rId17" xr:uid="{0FC6BF4E-B3F7-4B10-8F3D-F4990499FCDC}"/>
-    <hyperlink ref="H13" r:id="rId18" xr:uid="{5B927924-9F42-4FC1-A54D-3FA96B6BE0F8}"/>
-    <hyperlink ref="H14" r:id="rId19" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B226MOJVPNE/11487778" xr:uid="{261B60BF-E7B9-412E-ADE9-39C9C22F5694}"/>
-    <hyperlink ref="H4" r:id="rId20" xr:uid="{A3B9EFD3-1AE1-432D-A046-EB69FFDD8413}"/>
-    <hyperlink ref="H7" r:id="rId21" xr:uid="{A8C64BFE-52FE-4913-BF99-4ABD728FEB84}"/>
-    <hyperlink ref="H9" r:id="rId22" xr:uid="{866C3AA0-47E7-4D34-B47F-E2C9626259D5}"/>
-    <hyperlink ref="H8" r:id="rId23" xr:uid="{42BC71AF-2E36-45CB-9A55-C1B1ECA63DD6}"/>
+    <hyperlink ref="H13" r:id="rId17" xr:uid="{5B927924-9F42-4FC1-A54D-3FA96B6BE0F8}"/>
+    <hyperlink ref="H14" r:id="rId18" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL32B226MOJVPNE/11487778" xr:uid="{261B60BF-E7B9-412E-ADE9-39C9C22F5694}"/>
+    <hyperlink ref="H7" r:id="rId19" xr:uid="{A8C64BFE-52FE-4913-BF99-4ABD728FEB84}"/>
+    <hyperlink ref="H9" r:id="rId20" xr:uid="{866C3AA0-47E7-4D34-B47F-E2C9626259D5}"/>
+    <hyperlink ref="H8" r:id="rId21" xr:uid="{42BC71AF-2E36-45CB-9A55-C1B1ECA63DD6}"/>
+    <hyperlink ref="H12" r:id="rId22" xr:uid="{10D4338B-26FF-4D3A-B8B8-B02388C4D37D}"/>
+    <hyperlink ref="H4" r:id="rId23" xr:uid="{5C4B38ED-C91A-4163-A969-A22C81A5A599}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId24"/>

</xml_diff>